<commit_message>
got the request to work for a small dataset (2)
</commit_message>
<xml_diff>
--- a/conf/feature_referential_wellconnect.xlsx
+++ b/conf/feature_referential_wellconnect.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="variable_information" sheetId="1" state="visible" r:id="rId3"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="104">
   <si>
     <t xml:space="preserve">variable_name</t>
   </si>
@@ -47,10 +47,10 @@
     <t xml:space="preserve">variable_distrib</t>
   </si>
   <si>
-    <t xml:space="preserve">ParticipantID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unique identifier for each study participant</t>
+    <t xml:space="preserve">PHQ9_q1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PHQ-9 Question 1: “Little interest or pleasure in doing things” (0 = Not at all…3 = Nearly every day)</t>
   </si>
   <si>
     <t xml:space="preserve">Numeric</t>
@@ -59,58 +59,52 @@
     <t xml:space="preserve">int</t>
   </si>
   <si>
-    <t xml:space="preserve">PHQ-9-q1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PHQ-9 Question 1: “Little interest or pleasure in doing things” (0 = Not at all…3 = Nearly every day)</t>
-  </si>
-  <si>
     <t xml:space="preserve">0-3</t>
   </si>
   <si>
-    <t xml:space="preserve">PHQ-9-q2</t>
+    <t xml:space="preserve">PHQ9_q2</t>
   </si>
   <si>
     <t xml:space="preserve">PHQ-9 Question 2: “Feeling down, depressed, or hopeless”</t>
   </si>
   <si>
-    <t xml:space="preserve">PHQ-9-q3</t>
+    <t xml:space="preserve">PHQ9_q3</t>
   </si>
   <si>
     <t xml:space="preserve">PHQ-9 Question 3: “Trouble falling or staying asleep, or sleeping too much”</t>
   </si>
   <si>
-    <t xml:space="preserve">PHQ-9-q4</t>
+    <t xml:space="preserve">PHQ9_q4</t>
   </si>
   <si>
     <t xml:space="preserve">PHQ-9 Question 4: “Feeling tired or having little energy”</t>
   </si>
   <si>
-    <t xml:space="preserve">PHQ-9-q5</t>
+    <t xml:space="preserve">PHQ9_q5</t>
   </si>
   <si>
     <t xml:space="preserve">PHQ-9 Question 5: “Poor appetite or overeating”</t>
   </si>
   <si>
-    <t xml:space="preserve">PHQ-9-q6</t>
+    <t xml:space="preserve">PHQ9_q6</t>
   </si>
   <si>
     <t xml:space="preserve">PHQ-9 Question 6: “Feeling bad about yourself—or that you are a failure or have let yourself or your family down”</t>
   </si>
   <si>
-    <t xml:space="preserve">PHQ-9-q7</t>
+    <t xml:space="preserve">PHQ9_q7</t>
   </si>
   <si>
     <t xml:space="preserve">PHQ-9 Question 7: “Trouble concentrating on things (e.g., reading, watching TV)”</t>
   </si>
   <si>
-    <t xml:space="preserve">PHQ-9-q8</t>
+    <t xml:space="preserve">PHQ9_q8</t>
   </si>
   <si>
     <t xml:space="preserve">PHQ-9 Question 8: “Moving or speaking so slowly that other people could notice—or the opposite, being so fidgety or restless that you have been moving a lot more than usual”</t>
   </si>
   <si>
-    <t xml:space="preserve">PHQ-9-q9</t>
+    <t xml:space="preserve">PHQ9_q9</t>
   </si>
   <si>
     <t xml:space="preserve">PHQ-9 Question 9: “Thoughts that you would be better off dead or of hurting yourself in some way”</t>
@@ -164,7 +158,7 @@
     <t xml:space="preserve">Geen opleiding; Basisonderwijs; Vmbo/Mavo; Havo/Vwo; Mbo (niveau 1-4); HBO; Universiteit (Bachelor, Master, of hoger); Anders (specificeer): __________</t>
   </si>
   <si>
-    <t xml:space="preserve">CountryOFBirth</t>
+    <t xml:space="preserve">CountryOfBirth</t>
   </si>
   <si>
     <t xml:space="preserve">Country where participant was born</t>
@@ -182,13 +176,13 @@
     <t xml:space="preserve">Open text or list</t>
   </si>
   <si>
-    <t xml:space="preserve">CountryOFBirthMother</t>
+    <t xml:space="preserve">CountryOfBirthMother</t>
   </si>
   <si>
     <t xml:space="preserve">Mother’s country of birth</t>
   </si>
   <si>
-    <t xml:space="preserve">CountryOFBirthFather</t>
+    <t xml:space="preserve">CountryOfBirthFather</t>
   </si>
   <si>
     <t xml:space="preserve">Father’s country of birth</t>
@@ -257,13 +251,13 @@
     <t xml:space="preserve">Personality test Big Five component Neuroticism as measured by a condensed TIPI (Ten Item Personality Measure) questionnaire</t>
   </si>
   <si>
-    <t xml:space="preserve">TIPI_Oopenness</t>
+    <t xml:space="preserve">TIPI_Openness</t>
   </si>
   <si>
     <t xml:space="preserve">Personality test Big Five component Openness to experience as measured by a condensed TIPI (Ten Item Personality Measure) questionnaire</t>
   </si>
   <si>
-    <t xml:space="preserve">PANCRS-Affirmation</t>
+    <t xml:space="preserve">PANCRS_Affirmation</t>
   </si>
   <si>
     <t xml:space="preserve">Average agreement with items reflecting how much friends offer emotional support and validation when discussing problems (e.g. “My friend lets me know I’m not alone in how I feel”).</t>
@@ -272,76 +266,73 @@
     <t xml:space="preserve">1.0-5.0</t>
   </si>
   <si>
-    <t xml:space="preserve">PANCRS-ProblemSolving</t>
+    <t xml:space="preserve">PANCRS_ProblemSolving</t>
   </si>
   <si>
     <t xml:space="preserve">Average agreement with items reflecting collaborative problem-solving talk (e.g. “We brainstorm ways to fix what’s bothering me”).</t>
   </si>
   <si>
-    <t xml:space="preserve">PANCRS-EnhancingFriendship</t>
+    <t xml:space="preserve">PANCRS_EnhancingFriendship</t>
   </si>
   <si>
     <t xml:space="preserve">Average agreement with items reflecting how co-rumination strengthens the friendship bond (e.g. “Talking with my friend about problems makes us feel closer”).</t>
   </si>
   <si>
-    <t xml:space="preserve">PANCRS-TotalPositive</t>
+    <t xml:space="preserve">PANCRS_TotalPositive</t>
   </si>
   <si>
     <t xml:space="preserve">Mean of the three positive co-rumination subscales (Affirmation, ProblemSolving, EnhancingFriendship).</t>
   </si>
   <si>
-    <t xml:space="preserve">PANCRS-WorryAboutEvaluation</t>
+    <t xml:space="preserve">PANCRS_WorryAboutEvaluation</t>
   </si>
   <si>
     <t xml:space="preserve">Average agreement with items reflecting concern over being judged by friends (e.g. “I worry that my friend thinks less of me when I share my problems”).</t>
   </si>
   <si>
-    <t xml:space="preserve">PANCRS-InhibitingHappiness</t>
+    <t xml:space="preserve">PANCRS_InhibitingHappiness</t>
   </si>
   <si>
     <t xml:space="preserve">Average agreement with items reflecting how co-rumination dampens positive emotions (e.g. “When we talk about problems, I find it hard to feel happy even later”).</t>
   </si>
   <si>
-    <t xml:space="preserve">PANCRS-WorryAboutImpact</t>
+    <t xml:space="preserve">PANCRS_WorryAboutImpact</t>
   </si>
   <si>
     <t xml:space="preserve">Average agreement with items reflecting anxiety about one’s problems burdening friends (e.g. “I worry that my friend gets upset hearing about my issues”).</t>
   </si>
   <si>
-    <t xml:space="preserve">PANCRS-Slack</t>
+    <t xml:space="preserve">PANCRS_Slack</t>
   </si>
   <si>
     <t xml:space="preserve">Average agreement with items reflecting unhelpful or stuck conversation patterns (e.g. “Our talk goes over the same concerns without moving forward”).</t>
   </si>
   <si>
-    <t xml:space="preserve">PANCRS-TotalNegative</t>
+    <t xml:space="preserve">PANCRS_TotalNegative</t>
   </si>
   <si>
     <t xml:space="preserve">Mean of the four negative co-rumination subscales (WorryAboutEvaluation, InhibitingHappiness, WorryAboutImpact, Slack).</t>
   </si>
   <si>
-    <t xml:space="preserve">PANCRS-FrequencyPositive</t>
+    <t xml:space="preserve">PANCRS_FrequencyPositive</t>
   </si>
   <si>
     <t xml:space="preserve">Average reported frequency (e.g. 1=never…5=very often) of engaging in positive co-rumination behaviors (Affirmation, ProblemSolving, EnhancingFriendship).</t>
   </si>
   <si>
-    <t xml:space="preserve">PANCRS-FrequencyNegative</t>
+    <t xml:space="preserve">PANCRS_FrequencyNegative</t>
   </si>
   <si>
     <t xml:space="preserve">Average reported frequency of engaging in negative co-rumination behaviors (WorryAboutEvaluation, InhibitingHappiness, WorryAboutImpact, Slack).</t>
   </si>
   <si>
-    <t xml:space="preserve">PANCRS-TotalFrequency</t>
+    <t xml:space="preserve">PANCRS_TotalFrequency</t>
   </si>
   <si>
     <t xml:space="preserve">Mean of the FrequencyPositive and FrequencyNegative scores, reflecting overall co-rumination frequency.</t>
   </si>
   <si>
     <t xml:space="preserve">to_use_for_modelling</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WorkStatus</t>
   </si>
 </sst>
 </file>
@@ -425,7 +416,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -440,14 +431,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -644,8 +627,8 @@
   </sheetPr>
   <dimension ref="A1:I1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F20" activeCellId="0" sqref="F20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -688,7 +671,7 @@
       </c>
       <c r="I1" s="2"/>
     </row>
-    <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -701,13 +684,16 @@
       <c r="F2" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G2" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>10</v>
@@ -716,10 +702,10 @@
         <v>11</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
@@ -733,10 +719,10 @@
         <v>11</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
@@ -750,7 +736,7 @@
         <v>11</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -767,10 +753,10 @@
         <v>11</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
@@ -784,10 +770,10 @@
         <v>11</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>23</v>
       </c>
@@ -801,10 +787,10 @@
         <v>11</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>25</v>
       </c>
@@ -818,10 +804,10 @@
         <v>11</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
         <v>27</v>
       </c>
@@ -835,10 +821,10 @@
         <v>11</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
         <v>29</v>
       </c>
@@ -852,24 +838,21 @@
         <v>11</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" s="3" t="s">
         <v>32</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -880,95 +863,98 @@
         <v>35</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>11</v>
+        <v>37</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="F14" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="G14" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -979,13 +965,13 @@
         <v>54</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -996,95 +982,95 @@
         <v>56</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="3" t="s">
         <v>64</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>37</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B24" s="3" t="s">
         <v>66</v>
       </c>
+      <c r="B24" s="1" t="s">
+        <v>67</v>
+      </c>
       <c r="C24" s="1" t="s">
-        <v>38</v>
+        <v>10</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>39</v>
+        <v>68</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F25" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="G25" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1098,10 +1084,10 @@
         <v>10</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1115,10 +1101,10 @@
         <v>10</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1132,233 +1118,217 @@
         <v>10</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" s="3" t="s">
         <v>79</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G30" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B30" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="31" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B31" s="3" t="s">
         <v>84</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B32" s="3" t="s">
         <v>86</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B33" s="3" t="s">
         <v>88</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B34" s="3" t="s">
         <v>90</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B35" s="3" t="s">
         <v>92</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B36" s="3" t="s">
         <v>94</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B37" s="3" t="s">
         <v>96</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="B38" s="3" t="s">
         <v>98</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="B39" s="3" t="s">
         <v>100</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="B40" s="3" t="s">
         <v>102</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="G41" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
@@ -1379,36 +1349,36 @@
   </sheetPr>
   <dimension ref="A1:B41"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A41" activeCellId="0" sqref="A41"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A23" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C25" activeCellId="0" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.48"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>105</v>
+      <c r="B1" s="2" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B3" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1416,7 +1386,7 @@
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1424,7 +1394,7 @@
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1432,7 +1402,7 @@
       <c r="A6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1440,7 +1410,7 @@
       <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="B7" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1448,7 +1418,7 @@
       <c r="A8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="0" t="n">
+      <c r="B8" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1456,7 +1426,7 @@
       <c r="A9" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="0" t="n">
+      <c r="B9" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1464,7 +1434,7 @@
       <c r="A10" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="0" t="n">
+      <c r="B10" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1472,15 +1442,15 @@
       <c r="A11" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="0" t="n">
+      <c r="B11" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="B12" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1488,79 +1458,79 @@
       <c r="A13" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="0" t="n">
+      <c r="B13" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B14" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="B14" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B15" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="B15" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B16" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="B16" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B17" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="B17" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B18" s="0" t="n">
+        <v>51</v>
+      </c>
+      <c r="B18" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B19" s="0" t="n">
+        <v>53</v>
+      </c>
+      <c r="B19" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B20" s="0" t="n">
+        <v>55</v>
+      </c>
+      <c r="B20" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B21" s="0" t="n">
+        <v>58</v>
+      </c>
+      <c r="B21" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B22" s="0" t="n">
+        <v>61</v>
+      </c>
+      <c r="B22" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1568,119 +1538,119 @@
       <c r="A23" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B23" s="0" t="n">
+      <c r="B23" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="B24" s="0" t="n">
+        <v>66</v>
+      </c>
+      <c r="B24" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B25" s="0" t="n">
+        <v>70</v>
+      </c>
+      <c r="B25" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B26" s="0" t="n">
+        <v>72</v>
+      </c>
+      <c r="B26" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B27" s="0" t="n">
+        <v>74</v>
+      </c>
+      <c r="B27" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B28" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B29" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B29" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B30" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>81</v>
+      </c>
+      <c r="B30" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B31" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="36.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="B32" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="36.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="B33" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="B34" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="B35" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="B36" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="B37" s="0" t="n">
+      <c r="B37" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1688,33 +1658,28 @@
       <c r="A38" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="B38" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="B39" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="B40" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="B41" s="0" t="n">
-        <v>1</v>
-      </c>
+      <c r="B40" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B41" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>